<commit_message>
All type of personalities with fuzzy rules.
</commit_message>
<xml_diff>
--- a/EmotionRegulation/EmotionRegulationAsset/Results/.xlsx
+++ b/EmotionRegulation/EmotionRegulationAsset/Results/.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R140c24d76f284499"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R92e4c2f8b70240ff"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -38,16 +38,16 @@
     <x:t xml:space="preserve"> DOMINANT PERSONALITY </x:t>
   </x:si>
   <x:si>
-    <x:t>Distress</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bye</x:t>
+    <x:t>Hate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fired</x:t>
   </x:si>
   <x:si>
     <x:t>None</x:t>
   </x:si>
   <x:si>
-    <x:t>Middle Conscientiousness</x:t>
+    <x:t>High Conscientiousness</x:t>
   </x:si>
   <x:si>
     <x:t>Low Extraversion</x:t>
@@ -59,7 +59,7 @@
     <x:t>Low Agreeableness</x:t>
   </x:si>
   <x:si>
-    <x:t>Middle Openness</x:t>
+    <x:t>Low Openness</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -424,13 +424,13 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>-2.4000000953674316</x:v>
+        <x:v>-1.6607036590576172</x:v>
       </x:c>
       <x:c r="B2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>8</x:v>
+        <x:v>5.347113132476807</x:v>
       </x:c>
       <x:c r="D2" t="s">
         <x:v>9</x:v>

</xml_diff>